<commit_message>
Update LoginTest: switch-case klasik agar compile di Java 8+
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/LoginData.xlsx
+++ b/src/test/resources/Data/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\Project-Assigment-day-28\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D036739E-574A-4DE3-ABAE-27CFCC89AD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16D5DA8-7A5A-41CD-A7F7-D36C0D4B33E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>